<commit_message>
Updated Order & Testing
</commit_message>
<xml_diff>
--- a/documentation/Risk Assessment.xlsx
+++ b/documentation/Risk Assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\ims-demo\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423599CB-4880-4403-9E93-36C9F77E75A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC137DD-C1F5-4552-9788-61C92FBF1E9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{8CB24F64-C717-488D-A877-05C866C4B332}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Project Name:</t>
   </si>
@@ -128,6 +127,24 @@
   </si>
   <si>
     <t>Contract Covid-19 or a family member getting Covid-19</t>
+  </si>
+  <si>
+    <t>Schedule Risk</t>
+  </si>
+  <si>
+    <t>Not completing the project on time</t>
+  </si>
+  <si>
+    <t>Wrong time estimation
+ Resources are not tracked properly. All resources like staff, systems, skills of individuals, etc.
+ Failure to identify complex functionalities and time required to develop those functionalities.
+ Unexpected project scope expansions.</t>
+  </si>
+  <si>
+    <t>2 Weeks overall project sprint</t>
+  </si>
+  <si>
+    <t>On agile projects the team is heavily involved in planning and estimating through activities such as XP's planning game and Wideband Delphi workshops. By working in short increments the true velocity of the team quickly emerges and is visible to all stakeholders who are now more closely involved in the project. In short, the true progress is hard to hide and quickly revealed, giving feedback to the stakeholders.</t>
   </si>
 </sst>
 </file>
@@ -441,7 +458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -529,6 +546,15 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -574,13 +600,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -907,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672790C0-2960-4938-80FA-B969A373BC5B}">
   <dimension ref="A1:AM21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -982,11 +1005,11 @@
         <v>15</v>
       </c>
       <c r="E2" s="21"/>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="31" t="s">
         <v>29</v>
       </c>
       <c r="G2" s="23"/>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="33" t="s">
         <v>29</v>
       </c>
       <c r="I2" s="24"/>
@@ -1003,17 +1026,17 @@
       <c r="O2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="37" t="s">
+      <c r="P2" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="39"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="41"/>
+      <c r="W2" s="41"/>
+      <c r="X2" s="42"/>
     </row>
     <row r="3" spans="1:24" s="16" customFormat="1" ht="168.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
@@ -1030,12 +1053,12 @@
         <v>33</v>
       </c>
       <c r="E3" s="21"/>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="31" t="s">
         <v>29</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="21"/>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="32" t="s">
         <v>29</v>
       </c>
       <c r="J3" s="23"/>
@@ -1049,7 +1072,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:24" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:24" s="16" customFormat="1" ht="252" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <f t="shared" ref="A4:A21" si="0">A3+1</f>
         <v>3</v>
@@ -1057,17 +1080,31 @@
       <c r="B4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="21"/>
+      <c r="C4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="49" t="s">
+        <v>29</v>
+      </c>
       <c r="F4" s="22"/>
       <c r="G4" s="23"/>
       <c r="H4" s="21"/>
       <c r="I4" s="24"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="7"/>
+      <c r="J4" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="1:24" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
@@ -1125,17 +1162,17 @@
       <c r="O7" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="P7" s="33" t="s">
+      <c r="P7" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="33"/>
-      <c r="T7" s="33"/>
-      <c r="U7" s="33"/>
-      <c r="V7" s="33"/>
-      <c r="W7" s="33"/>
-      <c r="X7" s="34"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="36"/>
+      <c r="S7" s="36"/>
+      <c r="T7" s="36"/>
+      <c r="U7" s="36"/>
+      <c r="V7" s="36"/>
+      <c r="W7" s="36"/>
+      <c r="X7" s="37"/>
     </row>
     <row r="8" spans="1:24" ht="45.7" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
@@ -1157,17 +1194,17 @@
       <c r="O8" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="P8" s="35" t="s">
+      <c r="P8" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="35"/>
-      <c r="T8" s="35"/>
-      <c r="U8" s="35"/>
-      <c r="V8" s="35"/>
-      <c r="W8" s="35"/>
-      <c r="X8" s="36"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="38"/>
+      <c r="T8" s="38"/>
+      <c r="U8" s="38"/>
+      <c r="V8" s="38"/>
+      <c r="W8" s="38"/>
+      <c r="X8" s="39"/>
     </row>
     <row r="9" spans="1:24" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="4">
@@ -1189,17 +1226,17 @@
       <c r="O9" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="P9" s="35" t="s">
+      <c r="P9" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="35"/>
-      <c r="U9" s="35"/>
-      <c r="V9" s="35"/>
-      <c r="W9" s="35"/>
-      <c r="X9" s="36"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="38"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="38"/>
+      <c r="V9" s="38"/>
+      <c r="W9" s="38"/>
+      <c r="X9" s="39"/>
     </row>
     <row r="10" spans="1:24" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="4">
@@ -1239,17 +1276,17 @@
       <c r="O11" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="P11" s="40" t="s">
+      <c r="P11" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="40"/>
-      <c r="S11" s="40"/>
-      <c r="T11" s="40"/>
-      <c r="U11" s="40"/>
-      <c r="V11" s="40"/>
-      <c r="W11" s="40"/>
-      <c r="X11" s="41"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="43"/>
+      <c r="T11" s="43"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="43"/>
+      <c r="W11" s="43"/>
+      <c r="X11" s="44"/>
     </row>
     <row r="12" spans="1:24" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.95">
       <c r="A12" s="11">
@@ -1271,15 +1308,15 @@
       <c r="O12" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="42"/>
-      <c r="S12" s="42"/>
-      <c r="T12" s="42"/>
-      <c r="U12" s="42"/>
-      <c r="V12" s="42"/>
-      <c r="W12" s="42"/>
-      <c r="X12" s="43"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="45"/>
+      <c r="U12" s="45"/>
+      <c r="V12" s="45"/>
+      <c r="W12" s="45"/>
+      <c r="X12" s="46"/>
     </row>
     <row r="13" spans="1:24" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.95">
       <c r="A13" s="11">
@@ -1301,15 +1338,15 @@
       <c r="O13" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="P13" s="44"/>
-      <c r="Q13" s="44"/>
-      <c r="R13" s="44"/>
-      <c r="S13" s="44"/>
-      <c r="T13" s="44"/>
-      <c r="U13" s="44"/>
-      <c r="V13" s="44"/>
-      <c r="W13" s="44"/>
-      <c r="X13" s="45"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="47"/>
+      <c r="V13" s="47"/>
+      <c r="W13" s="47"/>
+      <c r="X13" s="48"/>
     </row>
     <row r="14" spans="1:24" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.95">
       <c r="A14" s="11">
@@ -1331,15 +1368,15 @@
       <c r="O14" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="P14" s="31"/>
-      <c r="Q14" s="31"/>
-      <c r="R14" s="31"/>
-      <c r="S14" s="31"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="31"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
-      <c r="X14" s="32"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
+      <c r="T14" s="34"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="34"/>
+      <c r="W14" s="34"/>
+      <c r="X14" s="35"/>
     </row>
     <row r="15" spans="1:24" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="11">
@@ -1488,21 +1525,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CB0BA5692D439F4BB79CC4D90864FB65" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5a0b4bc8ff41ed1b65ab69efcd88df2e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a228e58f-08c5-4e30-81dc-fb2ae1d06aa5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cccaba783f5d612f80b59805e7d0b95e" ns2:_="">
     <xsd:import namespace="a228e58f-08c5-4e30-81dc-fb2ae1d06aa5"/>
@@ -1680,24 +1702,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8350BFB4-A9D9-4E31-80BD-0DE15D9680ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADDABAF6-F01C-4289-9695-2F24BCAFA78E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26513C23-1B03-419F-B40E-B40C48D3FC52}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1713,4 +1733,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADDABAF6-F01C-4289-9695-2F24BCAFA78E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8350BFB4-A9D9-4E31-80BD-0DE15D9680ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>